<commit_message>
change default language to DE informal
</commit_message>
<xml_diff>
--- a/data_raw/MSA_dict.xlsx
+++ b/data_raw/MSA_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Drive\#3 - MSA package\MSA test package\MSA PsychTest R package\MSA\data_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Drive\#3 - MSA package\MSA test package\MSA_2.8.3\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2667E74-1207-4E4A-BEA4-9DB1C3FEB272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6007269-676C-4D3B-8C2A-9AC851CD3FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="186">
   <si>
     <t>key</t>
   </si>
@@ -690,6 +690,9 @@
     &lt;/div&gt;
        &lt;p&gt;Avant que la collecte de données ne commence, vous aurez l'opportunité d'entendre quelques exemples et de faire quelques essais pratiques. Cela vous aidera à mieux comprendre la tâche et à vous préparer pour le test réel.&lt;/p&gt;
 &lt;/body&gt;</t>
+  </si>
+  <si>
+    <t>de_inf</t>
   </si>
 </sst>
 </file>
@@ -787,8 +790,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -807,13 +810,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>23906</xdr:rowOff>
@@ -842,7 +845,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -863,7 +866,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -893,7 +896,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -916,9 +919,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -956,7 +959,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1062,7 +1065,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1212,21 +1215,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="123.7109375" customWidth="1"/>
-    <col min="3" max="4" width="150.5703125" customWidth="1"/>
-    <col min="5" max="5" width="123.7109375" customWidth="1"/>
+    <col min="3" max="5" width="150.5703125" customWidth="1"/>
+    <col min="6" max="6" width="123.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1237,13 +1240,16 @@
         <v>177</v>
       </c>
       <c r="D1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1257,10 +1263,13 @@
         <v>47</v>
       </c>
       <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -1274,10 +1283,13 @@
         <v>173</v>
       </c>
       <c r="E3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1285,16 +1297,19 @@
         <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1308,10 +1323,13 @@
         <v>17</v>
       </c>
       <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1319,16 +1337,19 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
         <v>103</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1336,16 +1357,19 @@
         <v>124</v>
       </c>
       <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
         <v>104</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>93</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1359,10 +1383,13 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1376,10 +1403,13 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1387,16 +1417,19 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>105</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1404,16 +1437,19 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" t="s">
         <v>106</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>94</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1421,16 +1457,19 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
         <v>107</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>59</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1444,10 +1483,13 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1455,16 +1497,19 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
         <v>108</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>60</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1478,10 +1523,13 @@
         <v>70</v>
       </c>
       <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1489,16 +1537,19 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
         <v>109</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>61</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1512,10 +1563,13 @@
         <v>21</v>
       </c>
       <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1529,10 +1583,13 @@
         <v>34</v>
       </c>
       <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1540,16 +1597,19 @@
         <v>85</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -1565,8 +1625,11 @@
       <c r="E20" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1582,8 +1645,11 @@
       <c r="E21" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1599,8 +1665,11 @@
       <c r="E22" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>165</v>
       </c>
@@ -1613,11 +1682,14 @@
       <c r="D23" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>166</v>
       </c>
@@ -1633,8 +1705,11 @@
       <c r="E24" s="6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F24" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1642,16 +1717,19 @@
         <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1659,16 +1737,19 @@
         <v>96</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1676,16 +1757,19 @@
         <v>125</v>
       </c>
       <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" t="s">
         <v>113</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>92</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1693,16 +1777,19 @@
         <v>126</v>
       </c>
       <c r="C28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" t="s">
         <v>114</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>99</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -1710,16 +1797,19 @@
         <v>127</v>
       </c>
       <c r="C29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" t="s">
         <v>115</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>100</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -1727,16 +1817,19 @@
         <v>128</v>
       </c>
       <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
         <v>116</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>101</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1744,16 +1837,19 @@
         <v>102</v>
       </c>
       <c r="C31" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" t="s">
         <v>117</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>118</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1767,10 +1863,13 @@
         <v>50</v>
       </c>
       <c r="E32" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1784,10 +1883,13 @@
         <v>51</v>
       </c>
       <c r="E33" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1795,16 +1897,19 @@
         <v>45</v>
       </c>
       <c r="C34" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" t="s">
         <v>120</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>119</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -1812,16 +1917,19 @@
         <v>57</v>
       </c>
       <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
         <v>121</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>56</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1829,16 +1937,19 @@
         <v>69</v>
       </c>
       <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
         <v>122</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>68</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1852,10 +1963,13 @@
         <v>75</v>
       </c>
       <c r="E37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -1863,16 +1977,19 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
         <v>123</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>72</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -1886,10 +2003,13 @@
         <v>73</v>
       </c>
       <c r="E39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>65</v>
       </c>
@@ -1903,10 +2023,13 @@
         <v>74</v>
       </c>
       <c r="E40" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -1920,10 +2043,13 @@
         <v>88</v>
       </c>
       <c r="E41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -1937,10 +2063,13 @@
         <v>91</v>
       </c>
       <c r="E42" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="393.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="393.75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>132</v>
       </c>
@@ -1948,41 +2077,44 @@
         <v>181</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="F43" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E45" s="3"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E52" s="4"/>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E54" s="3"/>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E56" s="3"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="3"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="4"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="3"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1990,14 +2122,16 @@
     <hyperlink ref="B20" r:id="rId1" xr:uid="{72C03BFD-2C2C-4707-8455-9A3685430207}"/>
     <hyperlink ref="B21" r:id="rId2" xr:uid="{2C3AE3AC-D225-4C7C-B120-2FAFB3C93CA5}"/>
     <hyperlink ref="B23" r:id="rId3" xr:uid="{189D53A6-5BED-420A-AA21-B45B532602A1}"/>
-    <hyperlink ref="C23" r:id="rId4" xr:uid="{6D9380BD-D329-4F17-AB89-CEAFD850206A}"/>
-    <hyperlink ref="D23" r:id="rId5" xr:uid="{60357076-1E21-4A27-917E-9EC72998F0AB}"/>
-    <hyperlink ref="C24" r:id="rId6" xr:uid="{8CC740FC-ED34-4EA6-BEC1-9755BB240220}"/>
-    <hyperlink ref="D24" r:id="rId7" xr:uid="{EB036BEC-9ACC-4F6B-9B4A-58C5412FBB8A}"/>
-    <hyperlink ref="E24" r:id="rId8" xr:uid="{74D081F7-7134-44DA-8150-E8559DD4009D}"/>
+    <hyperlink ref="D23" r:id="rId4" xr:uid="{6D9380BD-D329-4F17-AB89-CEAFD850206A}"/>
+    <hyperlink ref="E23" r:id="rId5" xr:uid="{60357076-1E21-4A27-917E-9EC72998F0AB}"/>
+    <hyperlink ref="D24" r:id="rId6" xr:uid="{8CC740FC-ED34-4EA6-BEC1-9755BB240220}"/>
+    <hyperlink ref="E24" r:id="rId7" xr:uid="{EB036BEC-9ACC-4F6B-9B4A-58C5412FBB8A}"/>
+    <hyperlink ref="F24" r:id="rId8" xr:uid="{74D081F7-7134-44DA-8150-E8559DD4009D}"/>
+    <hyperlink ref="C23" r:id="rId9" xr:uid="{68D1DA2F-3177-4E8B-B603-4BCF61687761}"/>
+    <hyperlink ref="C24" r:id="rId10" xr:uid="{2A84F79B-12E2-44DC-B16B-4EC0CDD4AC65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
-  <drawing r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <drawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix typo in instructions
</commit_message>
<xml_diff>
--- a/data_raw/MSA_dict.xlsx
+++ b/data_raw/MSA_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Drive\#3 - MSA package\MSA test package\MSA_2.8.3\data_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\My Drive\#3 - MSA package\MSA test package\MSA_2.8.5\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6007269-676C-4D3B-8C2A-9AC851CD3FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D817E2B-A6E6-4ED6-A15D-BC733E855E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MSA" sheetId="1" r:id="rId1"/>
@@ -275,11 +275,6 @@
   </si>
   <si>
     <t>INSTRUCTIONS_VIDEO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h4&gt;Welcome to the test for musical scene analysis (MSA)&lt;/h4&gt;  In this task, you will be presented with various music excerpts. Each music excerpt consists of two parts. In the first part a single instrument (lead voice, bass, guitar or piano) plays, in the second part a mixture of several instruments (mixture) plays. \\
-&lt;strong&gt; Your task is to decide whether the single target instrument played in the mixture of instruments. &lt;/strong&gt; \\
-Before the data collection begins, you will have the opportunity to hear some examples and do some practice trials. </t>
   </si>
   <si>
     <t>BUTTON_YES</t>
@@ -451,11 +446,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">In this task, you will be presented with various music excerpts. Each music excerpt consists of two parts. In the first part a single instrument (lead voice, bass, guitar or piano) plays, in the second part a mixture of several instruments (mixture) plays. \\ 
-&lt;strong&gt; Your task is to decide whether the single target instrument played in the mixture of instruments. &lt;/strong&gt; \\ By clicking on "Continue", the test begins and your responses will be saved.
-</t>
-  </si>
-  <si>
     <t>INSTRUCTIONS_LONG</t>
   </si>
   <si>
@@ -693,6 +683,16 @@
   </si>
   <si>
     <t>de_inf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this task, you will be presented with various music excerpts. Each music excerpt consists of two parts. In the first part a single instrument (lead voice, bass, guitar or piano) plays, in the second part a mixture of several instruments (mixture) plays. \\ 
+&lt;strong&gt; Your task is to decide whether the single target instrument is played in the mixture of instruments. &lt;/strong&gt; \\ By clicking on "Continue", the test begins and your responses will be saved.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h4&gt;Welcome to the test for musical scene analysis (MSA)&lt;/h4&gt;  In this task, you will be presented with various music excerpts. Each music excerpt consists of two parts. In the first part a single instrument (lead voice, bass, guitar or piano) plays, in the second part a mixture of several instruments (mixture) plays. \\
+&lt;strong&gt; Your task is to decide whether the single target instrument is played in the mixture of instruments. &lt;/strong&gt; \\
+Before the data collection begins, you will have the opportunity to hear some examples and do some practice trials. </t>
   </si>
 </sst>
 </file>
@@ -845,7 +845,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -896,7 +896,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1217,39 +1217,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="123.7109375" customWidth="1"/>
-    <col min="3" max="5" width="150.5703125" customWidth="1"/>
-    <col min="6" max="6" width="123.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.59765625" customWidth="1"/>
+    <col min="2" max="2" width="123.73046875" customWidth="1"/>
+    <col min="3" max="5" width="150.59765625" customWidth="1"/>
+    <col min="6" max="6" width="123.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1266,50 +1266,50 @@
         <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s">
         <v>172</v>
       </c>
-      <c r="C3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1326,10 +1326,10 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1340,36 +1340,36 @@
         <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
         <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1386,10 +1386,10 @@
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1406,10 +1406,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1417,19 +1417,19 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1437,19 +1437,19 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1460,16 +1460,16 @@
         <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" t="s">
         <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1486,10 +1486,10 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1500,16 +1500,16 @@
         <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E14" t="s">
         <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1526,10 +1526,10 @@
         <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1540,16 +1540,16 @@
         <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" t="s">
         <v>61</v>
       </c>
       <c r="F16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1566,10 +1566,10 @@
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1586,30 +1586,30 @@
         <v>34</v>
       </c>
       <c r="F18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>85</v>
+        <v>185</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1669,47 +1669,47 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B23" s="6" t="s">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>166</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>171</v>
-      </c>
       <c r="D24" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1717,139 +1717,139 @@
         <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>38</v>
       </c>
       <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F27" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F28" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F29" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F30" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D31" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" t="s">
         <v>117</v>
       </c>
-      <c r="E31" t="s">
-        <v>118</v>
-      </c>
       <c r="F31" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1866,10 +1866,10 @@
         <v>50</v>
       </c>
       <c r="F32" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1897,19 +1897,19 @@
         <v>45</v>
       </c>
       <c r="C34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" t="s">
         <v>119</v>
       </c>
-      <c r="D34" t="s">
-        <v>120</v>
-      </c>
       <c r="E34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F34" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -1920,16 +1920,16 @@
         <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E35" t="s">
         <v>56</v>
       </c>
       <c r="F35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1940,16 +1940,16 @@
         <v>68</v>
       </c>
       <c r="D36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E36" t="s">
         <v>68</v>
       </c>
       <c r="F36" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -1980,16 +1980,16 @@
         <v>72</v>
       </c>
       <c r="D38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E38" t="s">
         <v>72</v>
       </c>
       <c r="F38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -2006,10 +2006,10 @@
         <v>73</v>
       </c>
       <c r="F39" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>65</v>
       </c>
@@ -2026,94 +2026,94 @@
         <v>74</v>
       </c>
       <c r="F40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" t="s">
-        <v>88</v>
-      </c>
-      <c r="E41" t="s">
-        <v>88</v>
-      </c>
-      <c r="F41" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" t="s">
-        <v>91</v>
-      </c>
-      <c r="F42" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="393.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="362.25" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="D43" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="F45" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.45">
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.45">
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.45">
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.45">
       <c r="F52" s="4"/>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.45">
       <c r="F54" s="3"/>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.45">
       <c r="F56" s="3"/>
     </row>
   </sheetData>

</xml_diff>